<commit_message>
Updated benchmarks xls; wrapper to produce distr benchmarks hangs; new paper version
</commit_message>
<xml_diff>
--- a/src/generative_playground/molecules/nips_paper/benchmark_results.xlsx
+++ b/src/generative_playground/molecules/nips_paper/benchmark_results.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egork\Dropbox\GitHub\deep_games\generative_playground\src\generative_playground\molecules\nips_paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D320311-4CCB-4F8F-898E-3D6410634699}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65370074-34E3-47ED-B6BA-897970ABB11E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{8079D529-CDA9-4B38-8F52-B87D4603B0AF}"/>
+    <workbookView xWindow="14118" yWindow="0" windowWidth="8922" windowHeight="12360" xr2:uid="{8079D529-CDA9-4B38-8F52-B87D4603B0AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -102,7 +103,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -121,12 +122,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -140,12 +135,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,7 +457,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -503,8 +497,8 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="2">
-        <v>0.97899999999999998</v>
+      <c r="C2" s="1">
+        <v>0.999969</v>
       </c>
       <c r="D2">
         <v>0.99999970000000005</v>
@@ -606,8 +600,8 @@
       <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7" s="4">
-        <v>0.75</v>
+      <c r="C7" s="2">
+        <v>0.96099999999999997</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -630,7 +624,7 @@
         <v>0.998</v>
       </c>
       <c r="C8" s="2">
-        <v>0.99722</v>
+        <v>0.99741000000000002</v>
       </c>
       <c r="D8">
         <v>0.99918399999999996</v>

</xml_diff>

<commit_message>
Latest snapshot of benchmark results so far
</commit_message>
<xml_diff>
--- a/src/generative_playground/molecules/nips_paper/benchmark_results.xlsx
+++ b/src/generative_playground/molecules/nips_paper/benchmark_results.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egork\Dropbox\GitHub\deep_games\generative_playground\src\generative_playground\molecules\nips_paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65370074-34E3-47ED-B6BA-897970ABB11E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AB253A5D-FBBD-44DD-A5C9-F2C603C9C4D2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14118" yWindow="0" windowWidth="8922" windowHeight="12360" xr2:uid="{8079D529-CDA9-4B38-8F52-B87D4603B0AF}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" activeTab="1" xr2:uid="{8079D529-CDA9-4B38-8F52-B87D4603B0AF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Goal-oriented trivial" sheetId="1" r:id="rId1"/>
+    <sheet name="Distribution" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>Benchmark num</t>
   </si>
@@ -88,6 +89,33 @@
   </si>
   <si>
     <t>Our value calculated via benchmark</t>
+  </si>
+  <si>
+    <t>Validity</t>
+  </si>
+  <si>
+    <t>Uniqueness</t>
+  </si>
+  <si>
+    <t>Novelty</t>
+  </si>
+  <si>
+    <t>KL divergence</t>
+  </si>
+  <si>
+    <t>Frechet ChemNet distance</t>
+  </si>
+  <si>
+    <t>With discriminator</t>
+  </si>
+  <si>
+    <t>No priors</t>
+  </si>
+  <si>
+    <t>Unconditional priors</t>
+  </si>
+  <si>
+    <t>Conditional priors</t>
   </si>
 </sst>
 </file>
@@ -456,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37EAA091-637C-4FB4-9A4E-037A5F9C8221}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -581,7 +609,7 @@
         <v>0.94799999999999995</v>
       </c>
       <c r="C6" s="2">
-        <v>0.94579999999999997</v>
+        <v>0.94589000000000001</v>
       </c>
       <c r="D6">
         <v>0.9476</v>
@@ -601,7 +629,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="2">
-        <v>0.96099999999999997</v>
+        <v>0.98960000000000004</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -634,6 +662,95 @@
       </c>
       <c r="G8" t="s">
         <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FD7C084-A88D-4859-BD01-ACEEA1A3DF07}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="22.47265625" customWidth="1"/>
+    <col min="2" max="2" width="8.89453125" customWidth="1"/>
+    <col min="3" max="3" width="9.3125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0.99870000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4">
+        <v>0.98729999999999996</v>
+      </c>
+      <c r="E4">
+        <v>0.99460000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5">
+        <v>0.73</v>
+      </c>
+      <c r="E5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6">
+        <v>5.3100000000000001E-2</v>
+      </c>
+      <c r="E6">
+        <v>0.11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>